<commit_message>
excel report and all features bugs has fixed
</commit_message>
<xml_diff>
--- a/src/main/java/com/testdata/testdata.xlsx
+++ b/src/main/java/com/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkum1389\eclipse-workspace\Apollo_Dcotor_consult_prabhakar\src\main\java\com\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670AC28D-C9D7-42B4-91A2-3E136AEF79FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AEADEC-C9A4-475A-827D-B3B2A658C8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4120" yWindow="2810" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>contact</t>
+  </si>
+  <si>
+    <t>otp</t>
   </si>
 </sst>
 </file>
@@ -345,23 +348,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>8700042264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>